<commit_message>
added for path correction
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -3,39 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msira\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C412779-6EEE-440B-AC36-9E329C2E0309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7C2F6B53-D0B4-40CB-81D9-A7CE532CFB0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" activeTab="1" xr2:uid="{F29CD6D3-487F-49DB-BD3C-3FB247AFF38E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22464" windowHeight="7608" activeTab="1" xr2:uid="{F29CD6D3-487F-49DB-BD3C-3FB247AFF38E}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
     <sheet name="classEdit" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Scenario</t>
   </si>
@@ -124,9 +111,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>with valid data</t>
-  </si>
-  <si>
     <t>Micro service-01</t>
   </si>
   <si>
@@ -142,9 +126,6 @@
     <t>InActive</t>
   </si>
   <si>
-    <t>with invalid data</t>
-  </si>
-  <si>
     <t>SMPO-0001</t>
   </si>
   <si>
@@ -154,9 +135,6 @@
     <t>Kevin Thomas</t>
   </si>
   <si>
-    <t>with mandatory fields</t>
-  </si>
-  <si>
     <t>Python101</t>
   </si>
   <si>
@@ -169,9 +147,6 @@
     <t>Geetha takur</t>
   </si>
   <si>
-    <t>with ordinary fields</t>
-  </si>
-  <si>
     <t>Vidhya Test</t>
   </si>
   <si>
@@ -181,7 +156,7 @@
     <t>Getha  Takur</t>
   </si>
   <si>
-    <t>close cancel button</t>
+    <t>updateclass</t>
   </si>
 </sst>
 </file>
@@ -658,171 +633,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2500966A-FF5D-454E-AC22-110A1D442F7E}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>45711</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="2">
+        <v>45718</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2">
-        <v>45718</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E4" s="2">
+        <v>45712</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2">
+        <v>46441</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2">
         <v>45712</v>
       </c>
-      <c r="E4">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2">
-        <v>46441</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45712</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>48</v>
-      </c>
-    </row>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Batch data excel added
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayau\OneDrive\Desktop\LATEST GIT\Team9_AutomationSquad_LMS_UI_Hackathon_Phase2\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B501168-263A-40B6-A54C-D57A7BC9F2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1A2D89-35D7-4FA3-A3A1-07A34ACB57F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="600" windowWidth="29040" windowHeight="15000" xr2:uid="{F29CD6D3-487F-49DB-BD3C-3FB247AFF38E}"/>
+    <workbookView xWindow="2685" yWindow="3405" windowWidth="21600" windowHeight="10755" activeTab="1" xr2:uid="{F29CD6D3-487F-49DB-BD3C-3FB247AFF38E}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
+    <sheet name="Batch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Scenario</t>
   </si>
@@ -84,20 +85,83 @@
     <t>withoutRole</t>
   </si>
   <si>
-    <t>Feb@2023</t>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>BatchPrefix</t>
+  </si>
+  <si>
+    <t>BatchSuffix</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>NumberOfClasses</t>
+  </si>
+  <si>
+    <t>invalidSuffix</t>
+  </si>
+  <si>
+    <t>defg</t>
+  </si>
+  <si>
+    <t>invalidPrefix</t>
+  </si>
+  <si>
+    <t>tref</t>
+  </si>
+  <si>
+    <t>mandatoryFields</t>
+  </si>
+  <si>
+    <t>TestDef</t>
+  </si>
+  <si>
+    <t>testCase</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>oneFieldBlank</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>testcases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +186,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1CC4D1-8596-4996-9DF6-EB8DE85CCB61}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,8 +563,8 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -551,6 +615,132 @@
       </c>
       <c r="C8" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7A6BE3-1902-4097-8DFF-407E8CB79410}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>4567</v>
+      </c>
+      <c r="D4">
+        <v>6384</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>4567</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>